<commit_message>
2020 09 18 CJ
</commit_message>
<xml_diff>
--- a/src/main/resources/static/福利导入模板.xlsx
+++ b/src/main/resources/static/福利导入模板.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>工号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -33,7 +33,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>000962</t>
+    <t>名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020-09</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>130259</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>年终奖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>十三薪</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -41,11 +65,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2020-09</t>
+    <t>备注：半年奖+年终奖=奖金；除了奖金，十三薪，其他的都是福利；</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>半年奖</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -53,7 +77,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,6 +90,13 @@
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -89,12 +120,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -375,19 +409,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="3" width="9" style="2"/>
     <col min="4" max="4" width="17.875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="75.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -395,66 +430,102 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1">
-        <v>100</v>
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:6">
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:6">
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:6">
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:6">
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:6">
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:6">
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:6">
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:6">
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:6">
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:6">
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="4:4">

</xml_diff>